<commit_message>
(01) About Us added in FAQs (02) Added FAQ_page 4
</commit_message>
<xml_diff>
--- a/aura/assets/faq.xls.xlsx
+++ b/aura/assets/faq.xls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>sgn</t>
   </si>
@@ -113,105 +113,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>4)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Choose to pay by GPay / PayTM / Cash</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>5)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Open GPay/ PayTM app &amp; pay the amount</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Merchant verifies your payment &amp; confirms</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>7)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Once confirmed, the items will be delivered</t>
-    </r>
-  </si>
-  <si>
-    <t>Mention "Order No" in description</t>
-  </si>
-  <si>
     <t xml:space="preserve"> the order. You get a msg when confirmed.</t>
   </si>
   <si>
-    <t>your order in a few hours. For Cash payment</t>
-  </si>
-  <si>
-    <t>merchant confirms your order &amp; collects</t>
-  </si>
-  <si>
-    <t>bill amount while delivering the items.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -627,13 +531,154 @@
   </si>
   <si>
     <t>Want to buy more quantities?</t>
+  </si>
+  <si>
+    <t>We are serving authentic Tamil Brahmin</t>
+  </si>
+  <si>
+    <t>style food. No Onion / Garlic. We deliver</t>
+  </si>
+  <si>
+    <t>both BreakFast &amp; Lunch daily btwn</t>
+  </si>
+  <si>
+    <t>7:00am - 8:30am. Marathahalli as center of</t>
+  </si>
+  <si>
+    <t>point we server South East &amp; North West for</t>
+  </si>
+  <si>
+    <t>NS Mani Iyer: +91 97419 83633</t>
+  </si>
+  <si>
+    <t>Santosh Iyer: +91 93437 71700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a radius of around 10kms. </t>
+  </si>
+  <si>
+    <t>Beyond 10 KM a nominal delivery charge</t>
+  </si>
+  <si>
+    <t>will be applicable. Outdoor catering is also undertaken</t>
+  </si>
+  <si>
+    <t>We serve authentic Tamil Brahmin style food.</t>
+  </si>
+  <si>
+    <t>North West with Marathahalli as center point.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We undertake </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>outdoor catering</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> too.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">But we expect a minimum order for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>₹ 120.</t>
+    </r>
+  </si>
+  <si>
+    <t>If not, there will be a min delivery charge.</t>
+  </si>
+  <si>
+    <t>No onion / garlic. We deliver both BreakFast,</t>
+  </si>
+  <si>
+    <t>We serve around 10kms radius South East &amp;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lunch daily between </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7:00am - 8:30am</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>For free Delivery:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2) You shall place a minimum order for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>₹ 120.</t>
+    </r>
+  </si>
+  <si>
+    <t>Please share this in your Social Meida.</t>
+  </si>
+  <si>
+    <t>1) You shall be in 10kms radius South East or</t>
+  </si>
+  <si>
+    <t>NS Mani Iyer: 97419 83633, 93437 71700</t>
+  </si>
+  <si>
+    <t>https://t.me/ManiMama_Bot</t>
+  </si>
+  <si>
+    <t>Mani Iyer's Kitchen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -676,14 +721,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
       <name val="Arial"/>
@@ -693,6 +730,36 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -741,10 +808,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -753,9 +821,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -768,8 +833,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1048,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H7" sqref="H7:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1080,43 +1164,51 @@
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -1126,187 +1218,247 @@
         <v>18</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>40</v>
+      <c r="D12" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="H20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="H21" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="H22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="F19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H22" s="5"/>
+      <c r="I22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H23" s="6"/>
+      <c r="I23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="I24" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H30" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H32" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H33" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H34" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>